<commit_message>
2 messages removed while fixing #185
</commit_message>
<xml_diff>
--- a/RiseClipseValidatorSCLMessages.xlsx
+++ b/RiseClipseValidatorSCLMessages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcadet/git/RiseClipse/GitHub/riseclipse-validator-scl2003/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1584EC-FD3E-EF49-9213-39D1064A8F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAEFB5F-63E9-094F-A2DB-E9783CD56887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="660" windowWidth="36300" windowHeight="27680" xr2:uid="{D58BF774-7A59-3C48-B3D5-ECB80F73968C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$C$139</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$C$137</definedName>
   </definedNames>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="143">
   <si>
     <t>NSD/Validation</t>
   </si>
@@ -176,9 +176,6 @@
     <t>no group in LNodeType id "yyy" with LNClass "zzz" has all elements in namespace "ppp"</t>
   </si>
   <si>
-    <t>unexpected DO name "xxx" in LNodeType id "yyy" in namespace "ppp"</t>
-  </si>
-  <si>
     <t>NSD/Validation/DataObject</t>
   </si>
   <si>
@@ -429,9 +426,6 @@
   </si>
   <si>
     <t>DO "xxx"" in LNodeType id = "yyy" is deprecated in "zzz" in namespace "ppp"</t>
-  </si>
-  <si>
-    <t>DO "xxx"" in LNodeType id = "yyy" has an unrecognized name in namespace "ppp"</t>
   </si>
   <si>
     <t>DAType id = "yyy" refers to deprecated ConstructedAttribute "xxx" in namespace "ppp"</t>
@@ -853,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F32A72-AC13-4647-A6BC-C931315F0D46}">
-  <dimension ref="A1:C137"/>
+  <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="150" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128:XFD128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,13 +861,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -895,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -906,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -972,7 +966,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -983,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -994,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1005,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1016,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1027,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1038,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1126,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1137,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1148,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1159,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1170,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1181,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1192,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1203,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1214,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1225,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1236,7 +1230,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1247,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1258,12 +1252,12 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
@@ -1274,7 +1268,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
@@ -1285,7 +1279,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
@@ -1296,7 +1290,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
@@ -1307,7 +1301,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -1318,7 +1312,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -1329,7 +1323,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
@@ -1340,7 +1334,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
@@ -1351,7 +1345,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -1362,7 +1356,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -1373,7 +1367,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
@@ -1384,7 +1378,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -1395,7 +1389,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
@@ -1406,7 +1400,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
@@ -1417,7 +1411,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
@@ -1428,7 +1422,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B52" t="s">
         <v>1</v>
@@ -1439,7 +1433,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
         <v>1</v>
@@ -1450,7 +1444,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
@@ -1461,7 +1455,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
         <v>1</v>
@@ -1472,7 +1466,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B56" t="s">
         <v>1</v>
@@ -1483,7 +1477,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B57" t="s">
         <v>1</v>
@@ -1494,7 +1488,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
@@ -1505,7 +1499,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
@@ -1516,7 +1510,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
@@ -1527,18 +1521,18 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
         <v>46</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
@@ -1549,7 +1543,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B63" t="s">
         <v>1</v>
@@ -1560,7 +1554,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
@@ -1571,29 +1565,29 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="B66" t="s">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
         <v>1</v>
@@ -1604,7 +1598,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
@@ -1615,7 +1609,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
@@ -1626,7 +1620,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
@@ -1637,7 +1631,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
@@ -1648,7 +1642,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
@@ -1659,7 +1653,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
@@ -1670,7 +1664,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
@@ -1681,7 +1675,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
@@ -1692,7 +1686,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B76" t="s">
         <v>1</v>
@@ -1703,7 +1697,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
@@ -1714,7 +1708,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B78" t="s">
         <v>1</v>
@@ -1725,18 +1719,18 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
         <v>87</v>
-      </c>
-      <c r="B79" t="s">
-        <v>1</v>
-      </c>
-      <c r="C79" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
@@ -1747,7 +1741,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
@@ -1758,7 +1752,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
@@ -1769,18 +1763,18 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
@@ -1791,7 +1785,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
@@ -1802,7 +1796,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
@@ -1813,7 +1807,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
@@ -1824,18 +1818,18 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
@@ -1846,7 +1840,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
@@ -1857,7 +1851,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B91" t="s">
         <v>1</v>
@@ -1868,24 +1862,24 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
         <v>96</v>
-      </c>
-      <c r="B92" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -1907,7 +1901,7 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -1918,18 +1912,18 @@
         <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>102</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B97" t="s">
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -1940,7 +1934,7 @@
         <v>4</v>
       </c>
       <c r="C98" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -1951,7 +1945,7 @@
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -1962,7 +1956,7 @@
         <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -1973,7 +1967,7 @@
         <v>4</v>
       </c>
       <c r="C101" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -1984,7 +1978,7 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -1995,12 +1989,12 @@
         <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="B104" t="s">
         <v>4</v>
@@ -2011,51 +2005,51 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B105" t="s">
         <v>4</v>
       </c>
       <c r="C105" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B106" t="s">
         <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>132</v>
+        <v>14</v>
       </c>
       <c r="B107" t="s">
         <v>4</v>
       </c>
       <c r="C107" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B108" t="s">
         <v>4</v>
       </c>
       <c r="C108" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B109" t="s">
         <v>4</v>
@@ -2066,7 +2060,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B110" t="s">
         <v>4</v>
@@ -2077,7 +2071,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B111" t="s">
         <v>4</v>
@@ -2088,7 +2082,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B112" t="s">
         <v>4</v>
@@ -2099,7 +2093,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B113" t="s">
         <v>4</v>
@@ -2110,7 +2104,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B114" t="s">
         <v>4</v>
@@ -2121,7 +2115,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B115" t="s">
         <v>4</v>
@@ -2132,7 +2126,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B116" t="s">
         <v>4</v>
@@ -2143,7 +2137,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B117" t="s">
         <v>4</v>
@@ -2154,7 +2148,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B118" t="s">
         <v>4</v>
@@ -2165,7 +2159,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B119" t="s">
         <v>4</v>
@@ -2176,7 +2170,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B120" t="s">
         <v>4</v>
@@ -2187,7 +2181,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B121" t="s">
         <v>4</v>
@@ -2198,7 +2192,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B122" t="s">
         <v>4</v>
@@ -2209,7 +2203,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B123" t="s">
         <v>4</v>
@@ -2220,7 +2214,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B124" t="s">
         <v>4</v>
@@ -2231,7 +2225,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B125" t="s">
         <v>4</v>
@@ -2242,7 +2236,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B126" t="s">
         <v>4</v>
@@ -2253,7 +2247,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B127" t="s">
         <v>4</v>
@@ -2264,118 +2258,96 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B128" t="s">
         <v>4</v>
       </c>
       <c r="C128" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="B129" t="s">
         <v>4</v>
       </c>
       <c r="C129" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="B130" t="s">
         <v>4</v>
       </c>
       <c r="C130" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="B131" t="s">
         <v>4</v>
       </c>
       <c r="C131" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="B132" t="s">
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B133" t="s">
         <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B134" t="s">
         <v>4</v>
       </c>
       <c r="C134" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B135" t="s">
         <v>4</v>
       </c>
       <c r="C135" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>96</v>
-      </c>
-      <c r="B136" t="s">
-        <v>4</v>
-      </c>
-      <c r="C136" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>96</v>
-      </c>
-      <c r="B137" t="s">
-        <v>4</v>
-      </c>
-      <c r="C137" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C139" xr:uid="{98F32A72-AC13-4647-A6BC-C931315F0D46}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C139">
-      <sortCondition ref="B1:B139"/>
+  <autoFilter ref="A1:C137" xr:uid="{98F32A72-AC13-4647-A6BC-C931315F0D46}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C137">
+      <sortCondition ref="B1:B137"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>